<commit_message>
Implemented DDT with SoftAssert for user registration and updated related pages, utils, and test data
</commit_message>
<xml_diff>
--- a/testdata/register_user.xlsx
+++ b/testdata/register_user.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumLearning\OpenCart1.1\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumLearning\DemoQa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09BB1B4-DFED-443B-8A03-5B4D8A63D35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF65457E-DDB0-429F-B009-B09D736158AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A74BF28C-13B3-448C-A368-528222B83AEA}"/>
   </bookViews>
@@ -36,41 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
-  <si>
-    <t>ahsan@gmail.com</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>ahsan1@gmail.com</t>
-  </si>
-  <si>
-    <t>ahsan2@gmail.com</t>
-  </si>
-  <si>
-    <t>ahsan3@gmail.com</t>
-  </si>
-  <si>
-    <t>Test@124</t>
-  </si>
-  <si>
-    <t>Test@125</t>
-  </si>
-  <si>
-    <t>Test@126</t>
-  </si>
-  <si>
-    <t>hafiz@123</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="30">
   <si>
     <t>hafiz@gmail.com</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -89,16 +59,73 @@
     <t>TestStatus</t>
   </si>
   <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Ahsan@1234</t>
+  </si>
+  <si>
+    <t>Atif</t>
+  </si>
+  <si>
+    <t>Muneeb</t>
+  </si>
+  <si>
+    <t>Mudassar</t>
+  </si>
+  <si>
+    <t>Abbas</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Afzal</t>
+  </si>
+  <si>
+    <t>Manzoor</t>
+  </si>
+  <si>
+    <t>Iqbal</t>
+  </si>
+  <si>
+    <t>Muhammad</t>
+  </si>
+  <si>
+    <t>Ahsan</t>
+  </si>
+  <si>
+    <t>Hafiz</t>
+  </si>
+  <si>
+    <t>hafiz_ahsan</t>
+  </si>
+  <si>
+    <t>hafiz_ahsan1</t>
+  </si>
+  <si>
+    <t>hafiz_ahsan2</t>
+  </si>
+  <si>
+    <t>hafiz_ahsan3</t>
+  </si>
+  <si>
+    <t>hafiz_ahsan4</t>
+  </si>
+  <si>
+    <t>Test Failed</t>
+  </si>
+  <si>
+    <t>Execution Error</t>
+  </si>
+  <si>
     <t>Test Passed</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Test Error</t>
-  </si>
-  <si>
-    <t>Test Failed</t>
   </si>
 </sst>
 </file>
@@ -170,7 +197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -179,6 +206,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,131 +548,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C58C19E-A2FA-497E-B1AB-BA3539971C70}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.140625"/>
-    <col min="2" max="3" customWidth="true" width="30.85546875"/>
-    <col min="4" max="4" customWidth="true" width="24.85546875"/>
-    <col min="5" max="5" customWidth="true" width="27.140625"/>
+    <col min="1" max="1" customWidth="true" width="20.140625"/>
+    <col min="2" max="2" customWidth="true" width="19.0"/>
+    <col min="3" max="3" customWidth="true" width="31.140625"/>
+    <col min="4" max="5" customWidth="true" width="30.85546875"/>
+    <col min="6" max="6" customWidth="true" width="24.85546875"/>
+    <col min="7" max="7" customWidth="true" width="27.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4">
+        <v>123457</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4">
+        <v>123458</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4">
+        <v>123459</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>16</v>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>17</v>
+      <c r="F7" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{2554BE62-58FB-4EF8-B4E9-BC7AA6F789A4}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{94C202B9-5B48-433F-AC5A-BB69184E37B1}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{620EE7DD-074D-4469-99B4-095164ED1462}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{0C892F10-2B92-44BA-8A0A-29861C7C1742}"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{9962B66F-159E-4FAD-9432-566F1DEDB140}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{2DF0986C-8FD2-4F0B-9B4E-AEBDE4C7F413}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>